<commit_message>
Added SQL command building macros to template sheets
</commit_message>
<xml_diff>
--- a/tools/RoatanClinics.xlsx
+++ b/tools/RoatanClinics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\bobw\Documents\GitHub\docsbydesign\piClinic\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{33BC1055-FB1B-431E-B486-11DD7FB54837}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F71DB1F-ABC6-4947-BEA3-F79697BA7E34}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="546" windowWidth="19158" windowHeight="11292" xr2:uid="{B050DA51-73D4-4A63-9D6D-7265F307B49B}"/>
+    <workbookView xWindow="3960" yWindow="636" windowWidth="19158" windowHeight="11292" xr2:uid="{B050DA51-73D4-4A63-9D6D-7265F307B49B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="35">
   <si>
     <t>thisClinic</t>
   </si>
@@ -133,14 +133,25 @@
   </si>
   <si>
     <t>Anneth Cooper</t>
+  </si>
+  <si>
+    <t>SQL Command</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -168,9 +179,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -485,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8646F3A-9A7C-4F23-973D-545219BDB1A0}">
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:AM4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+    <sheetView tabSelected="1" topLeftCell="AF1" workbookViewId="0">
+      <selection activeCell="AK2" sqref="AK2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -508,9 +520,10 @@
     <col min="15" max="15" width="10.26171875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.41796875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10.41796875" bestFit="1" customWidth="1"/>
+    <col min="19" max="38" width="8.83984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -562,8 +575,21 @@
       <c r="Q1" t="s">
         <v>16</v>
       </c>
+      <c r="S1" t="str">
+        <f>CONCATENATE("INSERT INTO `clinic` (`",A1,"`,`",B1,"`,`",C1,"`,`",D1,"`,`",E1,"`,`",F1,"`,`",G1,"`,`",H1,"`,`",I1,"`,`",J1,"`,`",K1,"`,`",L1,"`,`",M1,"`,`",N1,"`,`",O1,"`,`",P1,"`,`",Q1,"`) VALUES (")</f>
+        <v>INSERT INTO `clinic` (`thisClinic`,`publicID`,`typeCode`,`careLevel`,`longName`,`shortName`,`currency`,`address1`,`address2`,`clinicNeighborhood`,`clinicCity`,`clinicState`,`clinicRegion`,`clinicDirector`,`clinicService`,`modifiedDate`,`createdDate`) VALUES (</v>
+      </c>
+      <c r="AM1" s="2" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
       <c r="C2" t="s">
         <v>17</v>
       </c>
@@ -603,8 +629,87 @@
       <c r="Q2" t="s">
         <v>21</v>
       </c>
+      <c r="S2" t="str">
+        <f>IF(A2&lt;&gt;"",CONCATENATE("""",A2,""","),"NULL,")</f>
+        <v>"0",</v>
+      </c>
+      <c r="T2" t="str">
+        <f t="shared" ref="T2:AI2" si="0">IF(B2&lt;&gt;"",CONCATENATE("""",B2,""","),"NULL,")</f>
+        <v>"0",</v>
+      </c>
+      <c r="U2" t="str">
+        <f t="shared" si="0"/>
+        <v>"UAPS",</v>
+      </c>
+      <c r="V2" t="str">
+        <f t="shared" si="0"/>
+        <v>"Primario",</v>
+      </c>
+      <c r="W2" t="str">
+        <f t="shared" si="0"/>
+        <v>"Consolation Clinic",</v>
+      </c>
+      <c r="X2" t="str">
+        <f t="shared" si="0"/>
+        <v>"Consolation Clinic",</v>
+      </c>
+      <c r="Y2" t="str">
+        <f t="shared" si="0"/>
+        <v>"HNL",</v>
+      </c>
+      <c r="Z2" t="str">
+        <f t="shared" si="0"/>
+        <v>NULL,</v>
+      </c>
+      <c r="AA2" t="str">
+        <f t="shared" si="0"/>
+        <v>NULL,</v>
+      </c>
+      <c r="AB2" t="str">
+        <f t="shared" si="0"/>
+        <v>"Consolation Bight",</v>
+      </c>
+      <c r="AC2" t="str">
+        <f t="shared" si="0"/>
+        <v>"Roatan",</v>
+      </c>
+      <c r="AD2" t="str">
+        <f t="shared" si="0"/>
+        <v>"Islas de la Bahia",</v>
+      </c>
+      <c r="AE2" t="str">
+        <f t="shared" si="0"/>
+        <v>"11",</v>
+      </c>
+      <c r="AF2" t="str">
+        <f t="shared" si="0"/>
+        <v>"Aleynska Grant",</v>
+      </c>
+      <c r="AG2" t="str">
+        <f t="shared" si="0"/>
+        <v>"Outpatient",</v>
+      </c>
+      <c r="AH2" t="str">
+        <f>IF(P2&lt;&gt;"",CONCATENATE(P2,","),"NULL,")</f>
+        <v>NOW(),</v>
+      </c>
+      <c r="AI2" t="str">
+        <f>IF(Q2&lt;&gt;"",CONCATENATE(Q2),"NULL")</f>
+        <v>NOW()</v>
+      </c>
+      <c r="AK2" t="str">
+        <f>CONCATENATE(S2,T2,U2,V2,W2,X2,Y2,Z2,AA2,AB2,AC2,AD2,AE2,AF2,AG2,AH2,AI2,");")</f>
+        <v>"0","0","UAPS","Primario","Consolation Clinic","Consolation Clinic","HNL",NULL,NULL,"Consolation Bight","Roatan","Islas de la Bahia","11","Aleynska Grant","Outpatient",NOW(),NOW());</v>
+      </c>
+      <c r="AM2" t="str">
+        <f>CONCATENATE($S$1,AK2)</f>
+        <v>INSERT INTO `clinic` (`thisClinic`,`publicID`,`typeCode`,`careLevel`,`longName`,`shortName`,`currency`,`address1`,`address2`,`clinicNeighborhood`,`clinicCity`,`clinicState`,`clinicRegion`,`clinicDirector`,`clinicService`,`modifiedDate`,`createdDate`) VALUES ("0","0","UAPS","Primario","Consolation Clinic","Consolation Clinic","HNL",NULL,NULL,"Consolation Bight","Roatan","Islas de la Bahia","11","Aleynska Grant","Outpatient",NOW(),NOW());</v>
+      </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3">
+        <v>0</v>
+      </c>
       <c r="B3" s="1" t="s">
         <v>30</v>
       </c>
@@ -647,8 +752,90 @@
       <c r="Q3" t="s">
         <v>21</v>
       </c>
+      <c r="S3" t="str">
+        <f t="shared" ref="S3:S4" si="1">IF(A3&lt;&gt;"",CONCATENATE("""",A3,""","),"NULL,")</f>
+        <v>"0",</v>
+      </c>
+      <c r="T3" t="str">
+        <f t="shared" ref="T3:T4" si="2">IF(B3&lt;&gt;"",CONCATENATE("""",B3,""","),"NULL,")</f>
+        <v>"001348",</v>
+      </c>
+      <c r="U3" t="str">
+        <f t="shared" ref="U3:U4" si="3">IF(C3&lt;&gt;"",CONCATENATE("""",C3,""","),"NULL,")</f>
+        <v>"UAPS",</v>
+      </c>
+      <c r="V3" t="str">
+        <f t="shared" ref="V3:V4" si="4">IF(D3&lt;&gt;"",CONCATENATE("""",D3,""","),"NULL,")</f>
+        <v>"Primario",</v>
+      </c>
+      <c r="W3" t="str">
+        <f t="shared" ref="W3:W4" si="5">IF(E3&lt;&gt;"",CONCATENATE("""",E3,""","),"NULL,")</f>
+        <v>"Vasijas de Misericordia",</v>
+      </c>
+      <c r="X3" t="str">
+        <f t="shared" ref="X3:X4" si="6">IF(F3&lt;&gt;"",CONCATENATE("""",F3,""","),"NULL,")</f>
+        <v>"Vasijas de Misericordia",</v>
+      </c>
+      <c r="Y3" t="str">
+        <f t="shared" ref="Y3:Y4" si="7">IF(G3&lt;&gt;"",CONCATENATE("""",G3,""","),"NULL,")</f>
+        <v>"HNL",</v>
+      </c>
+      <c r="Z3" t="str">
+        <f t="shared" ref="Z3:Z4" si="8">IF(H3&lt;&gt;"",CONCATENATE("""",H3,""","),"NULL,")</f>
+        <v>NULL,</v>
+      </c>
+      <c r="AA3" t="str">
+        <f t="shared" ref="AA3:AA4" si="9">IF(I3&lt;&gt;"",CONCATENATE("""",I3,""","),"NULL,")</f>
+        <v>NULL,</v>
+      </c>
+      <c r="AB3" t="str">
+        <f t="shared" ref="AB3:AB4" si="10">IF(J3&lt;&gt;"",CONCATENATE("""",J3,""","),"NULL,")</f>
+        <v>"French Cay Harbour",</v>
+      </c>
+      <c r="AC3" t="str">
+        <f t="shared" ref="AC3:AC4" si="11">IF(K3&lt;&gt;"",CONCATENATE("""",K3,""","),"NULL,")</f>
+        <v>"Roatan",</v>
+      </c>
+      <c r="AD3" t="str">
+        <f t="shared" ref="AD3:AD4" si="12">IF(L3&lt;&gt;"",CONCATENATE("""",L3,""","),"NULL,")</f>
+        <v>"Islas de la Bahia",</v>
+      </c>
+      <c r="AE3" t="str">
+        <f t="shared" ref="AE3:AE4" si="13">IF(M3&lt;&gt;"",CONCATENATE("""",M3,""","),"NULL,")</f>
+        <v>"11",</v>
+      </c>
+      <c r="AF3" t="str">
+        <f t="shared" ref="AF3:AF4" si="14">IF(N3&lt;&gt;"",CONCATENATE("""",N3,""","),"NULL,")</f>
+        <v>"Dra. Sarai Raudales",</v>
+      </c>
+      <c r="AG3" t="str">
+        <f t="shared" ref="AG3:AG4" si="15">IF(O3&lt;&gt;"",CONCATENATE("""",O3,""","),"NULL,")</f>
+        <v>"Outpatient",</v>
+      </c>
+      <c r="AH3" t="str">
+        <f t="shared" ref="AH3:AH4" si="16">IF(P3&lt;&gt;"",CONCATENATE(P3,","),"NULL,")</f>
+        <v>NOW(),</v>
+      </c>
+      <c r="AI3" t="str">
+        <f t="shared" ref="AI3:AI4" si="17">IF(Q3&lt;&gt;"",CONCATENATE(Q3),"NULL")</f>
+        <v>NOW()</v>
+      </c>
+      <c r="AK3" t="str">
+        <f t="shared" ref="AK3:AK4" si="18">CONCATENATE(S3,T3,U3,V3,W3,X3,Y3,Z3,AA3,AB3,AC3,AD3,AE3,AF3,AG3,AH3,AI3,");")</f>
+        <v>"0","001348","UAPS","Primario","Vasijas de Misericordia","Vasijas de Misericordia","HNL",NULL,NULL,"French Cay Harbour","Roatan","Islas de la Bahia","11","Dra. Sarai Raudales","Outpatient",NOW(),NOW());</v>
+      </c>
+      <c r="AM3" t="str">
+        <f t="shared" ref="AM3:AM4" si="19">CONCATENATE($S$1,AK3)</f>
+        <v>INSERT INTO `clinic` (`thisClinic`,`publicID`,`typeCode`,`careLevel`,`longName`,`shortName`,`currency`,`address1`,`address2`,`clinicNeighborhood`,`clinicCity`,`clinicState`,`clinicRegion`,`clinicDirector`,`clinicService`,`modifiedDate`,`createdDate`) VALUES ("0","001348","UAPS","Primario","Vasijas de Misericordia","Vasijas de Misericordia","HNL",NULL,NULL,"French Cay Harbour","Roatan","Islas de la Bahia","11","Dra. Sarai Raudales","Outpatient",NOW(),NOW());</v>
+      </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
       <c r="C4" t="s">
         <v>17</v>
       </c>
@@ -687,6 +874,82 @@
       </c>
       <c r="Q4" t="s">
         <v>21</v>
+      </c>
+      <c r="S4" t="str">
+        <f t="shared" si="1"/>
+        <v>"0",</v>
+      </c>
+      <c r="T4" t="str">
+        <f t="shared" si="2"/>
+        <v>"0",</v>
+      </c>
+      <c r="U4" t="str">
+        <f t="shared" si="3"/>
+        <v>"UAPS",</v>
+      </c>
+      <c r="V4" t="str">
+        <f t="shared" si="4"/>
+        <v>"Primario",</v>
+      </c>
+      <c r="W4" t="str">
+        <f t="shared" si="5"/>
+        <v>"Oak Ridge Community Health Association",</v>
+      </c>
+      <c r="X4" t="str">
+        <f t="shared" si="6"/>
+        <v>"Oak Ridge Community Health Association",</v>
+      </c>
+      <c r="Y4" t="str">
+        <f t="shared" si="7"/>
+        <v>"HNL",</v>
+      </c>
+      <c r="Z4" t="str">
+        <f t="shared" si="8"/>
+        <v>NULL,</v>
+      </c>
+      <c r="AA4" t="str">
+        <f t="shared" si="9"/>
+        <v>NULL,</v>
+      </c>
+      <c r="AB4" t="str">
+        <f t="shared" si="10"/>
+        <v>"Oak Ridge",</v>
+      </c>
+      <c r="AC4" t="str">
+        <f t="shared" si="11"/>
+        <v>"Roatan",</v>
+      </c>
+      <c r="AD4" t="str">
+        <f t="shared" si="12"/>
+        <v>"Islas de la Bahia",</v>
+      </c>
+      <c r="AE4" t="str">
+        <f t="shared" si="13"/>
+        <v>"11",</v>
+      </c>
+      <c r="AF4" t="str">
+        <f t="shared" si="14"/>
+        <v>"Anneth Cooper",</v>
+      </c>
+      <c r="AG4" t="str">
+        <f t="shared" si="15"/>
+        <v>"Outpatient",</v>
+      </c>
+      <c r="AH4" t="str">
+        <f t="shared" si="16"/>
+        <v>NOW(),</v>
+      </c>
+      <c r="AI4" t="str">
+        <f t="shared" si="17"/>
+        <v>NOW()</v>
+      </c>
+      <c r="AK4" t="str">
+        <f t="shared" si="18"/>
+        <v>"0","0","UAPS","Primario","Oak Ridge Community Health Association","Oak Ridge Community Health Association","HNL",NULL,NULL,"Oak Ridge","Roatan","Islas de la Bahia","11","Anneth Cooper","Outpatient",NOW(),NOW());</v>
+      </c>
+      <c r="AM4" t="str">
+        <f t="shared" si="19"/>
+        <v>INSERT INTO `clinic` (`thisClinic`,`publicID`,`typeCode`,`careLevel`,`longName`,`shortName`,`currency`,`address1`,`address2`,`clinicNeighborhood`,`clinicCity`,`clinicState`,`clinicRegion`,`clinicDirector`,`clinicService`,`modifiedDate`,`createdDate`) VALUES ("0","0","UAPS","Primario","Oak Ridge Community Health Association","Oak Ridge Community Health Association","HNL",NULL,NULL,"Oak Ridge","Roatan","Islas de la Bahia","11","Anneth Cooper","Outpatient",NOW(),NOW());</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added roatanClinics script to load clinics
</commit_message>
<xml_diff>
--- a/tools/RoatanClinics.xlsx
+++ b/tools/RoatanClinics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\bobw\Documents\GitHub\docsbydesign\piClinic\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F71DB1F-ABC6-4947-BEA3-F79697BA7E34}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E260E21-D5A3-4BCF-8253-CB636E6CBA8D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3960" yWindow="636" windowWidth="19158" windowHeight="11292" xr2:uid="{B050DA51-73D4-4A63-9D6D-7265F307B49B}"/>
+    <workbookView xWindow="3882" yWindow="636" windowWidth="19158" windowHeight="11292" xr2:uid="{B050DA51-73D4-4A63-9D6D-7265F307B49B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -499,8 +499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8646F3A-9A7C-4F23-973D-545219BDB1A0}">
   <dimension ref="A1:AM4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AF1" workbookViewId="0">
-      <selection activeCell="AK2" sqref="AK2"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="AM2" sqref="AM2:AM4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -520,7 +520,7 @@
     <col min="15" max="15" width="10.26171875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.41796875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10.41796875" bestFit="1" customWidth="1"/>
-    <col min="19" max="38" width="8.83984375" customWidth="1"/>
+    <col min="19" max="38" width="8.83984375" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:39" x14ac:dyDescent="0.55000000000000004">
@@ -587,9 +587,6 @@
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
       <c r="C2" t="s">
         <v>17</v>
       </c>
@@ -634,8 +631,8 @@
         <v>"0",</v>
       </c>
       <c r="T2" t="str">
-        <f t="shared" ref="T2:AI2" si="0">IF(B2&lt;&gt;"",CONCATENATE("""",B2,""","),"NULL,")</f>
-        <v>"0",</v>
+        <f t="shared" ref="T2:AG2" si="0">IF(B2&lt;&gt;"",CONCATENATE("""",B2,""","),"NULL,")</f>
+        <v>NULL,</v>
       </c>
       <c r="U2" t="str">
         <f t="shared" si="0"/>
@@ -699,11 +696,11 @@
       </c>
       <c r="AK2" t="str">
         <f>CONCATENATE(S2,T2,U2,V2,W2,X2,Y2,Z2,AA2,AB2,AC2,AD2,AE2,AF2,AG2,AH2,AI2,");")</f>
-        <v>"0","0","UAPS","Primario","Consolation Clinic","Consolation Clinic","HNL",NULL,NULL,"Consolation Bight","Roatan","Islas de la Bahia","11","Aleynska Grant","Outpatient",NOW(),NOW());</v>
+        <v>"0",NULL,"UAPS","Primario","Consolation Clinic","Consolation Clinic","HNL",NULL,NULL,"Consolation Bight","Roatan","Islas de la Bahia","11","Aleynska Grant","Outpatient",NOW(),NOW());</v>
       </c>
       <c r="AM2" t="str">
         <f>CONCATENATE($S$1,AK2)</f>
-        <v>INSERT INTO `clinic` (`thisClinic`,`publicID`,`typeCode`,`careLevel`,`longName`,`shortName`,`currency`,`address1`,`address2`,`clinicNeighborhood`,`clinicCity`,`clinicState`,`clinicRegion`,`clinicDirector`,`clinicService`,`modifiedDate`,`createdDate`) VALUES ("0","0","UAPS","Primario","Consolation Clinic","Consolation Clinic","HNL",NULL,NULL,"Consolation Bight","Roatan","Islas de la Bahia","11","Aleynska Grant","Outpatient",NOW(),NOW());</v>
+        <v>INSERT INTO `clinic` (`thisClinic`,`publicID`,`typeCode`,`careLevel`,`longName`,`shortName`,`currency`,`address1`,`address2`,`clinicNeighborhood`,`clinicCity`,`clinicState`,`clinicRegion`,`clinicDirector`,`clinicService`,`modifiedDate`,`createdDate`) VALUES ("0",NULL,"UAPS","Primario","Consolation Clinic","Consolation Clinic","HNL",NULL,NULL,"Consolation Bight","Roatan","Islas de la Bahia","11","Aleynska Grant","Outpatient",NOW(),NOW());</v>
       </c>
     </row>
     <row r="3" spans="1:39" x14ac:dyDescent="0.55000000000000004">
@@ -833,9 +830,6 @@
       <c r="A4">
         <v>0</v>
       </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
       <c r="C4" t="s">
         <v>17</v>
       </c>
@@ -881,7 +875,7 @@
       </c>
       <c r="T4" t="str">
         <f t="shared" si="2"/>
-        <v>"0",</v>
+        <v>NULL,</v>
       </c>
       <c r="U4" t="str">
         <f t="shared" si="3"/>
@@ -945,11 +939,11 @@
       </c>
       <c r="AK4" t="str">
         <f t="shared" si="18"/>
-        <v>"0","0","UAPS","Primario","Oak Ridge Community Health Association","Oak Ridge Community Health Association","HNL",NULL,NULL,"Oak Ridge","Roatan","Islas de la Bahia","11","Anneth Cooper","Outpatient",NOW(),NOW());</v>
+        <v>"0",NULL,"UAPS","Primario","Oak Ridge Community Health Association","Oak Ridge Community Health Association","HNL",NULL,NULL,"Oak Ridge","Roatan","Islas de la Bahia","11","Anneth Cooper","Outpatient",NOW(),NOW());</v>
       </c>
       <c r="AM4" t="str">
         <f t="shared" si="19"/>
-        <v>INSERT INTO `clinic` (`thisClinic`,`publicID`,`typeCode`,`careLevel`,`longName`,`shortName`,`currency`,`address1`,`address2`,`clinicNeighborhood`,`clinicCity`,`clinicState`,`clinicRegion`,`clinicDirector`,`clinicService`,`modifiedDate`,`createdDate`) VALUES ("0","0","UAPS","Primario","Oak Ridge Community Health Association","Oak Ridge Community Health Association","HNL",NULL,NULL,"Oak Ridge","Roatan","Islas de la Bahia","11","Anneth Cooper","Outpatient",NOW(),NOW());</v>
+        <v>INSERT INTO `clinic` (`thisClinic`,`publicID`,`typeCode`,`careLevel`,`longName`,`shortName`,`currency`,`address1`,`address2`,`clinicNeighborhood`,`clinicCity`,`clinicState`,`clinicRegion`,`clinicDirector`,`clinicService`,`modifiedDate`,`createdDate`) VALUES ("0",NULL,"UAPS","Primario","Oak Ridge Community Health Association","Oak Ridge Community Health Association","HNL",NULL,NULL,"Oak Ridge","Roatan","Islas de la Bahia","11","Anneth Cooper","Outpatient",NOW(),NOW());</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Replaced roatan clinic script
</commit_message>
<xml_diff>
--- a/tools/RoatanClinics.xlsx
+++ b/tools/RoatanClinics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\bobw\Documents\GitHub\docsbydesign\piClinic\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E260E21-D5A3-4BCF-8253-CB636E6CBA8D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F2E3D96-60DD-4509-BD36-C15ECBA46CF1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3882" yWindow="636" windowWidth="19158" windowHeight="11292" xr2:uid="{B050DA51-73D4-4A63-9D6D-7265F307B49B}"/>
   </bookViews>
@@ -499,8 +499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8646F3A-9A7C-4F23-973D-545219BDB1A0}">
   <dimension ref="A1:AM4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="AM2" sqref="AM2:AM4"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="AM2" sqref="AM2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>